<commit_message>
Add support for enclosure door open sensor
</commit_message>
<xml_diff>
--- a/doc/wiring.xlsx
+++ b/doc/wiring.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -290,6 +290,21 @@
   </si>
   <si>
     <t>SDI data (#1)</t>
+  </si>
+  <si>
+    <t>Encl. door sensor</t>
+  </si>
+  <si>
+    <t>state detect</t>
+  </si>
+  <si>
+    <t>excitation</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
@@ -755,7 +770,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,6 +1104,18 @@
       <c r="D15" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="F15" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
@@ -1101,6 +1128,16 @@
       <c r="D16" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="F16" s="19"/>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
@@ -1391,7 +1428,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="F13:F14"/>
@@ -1406,6 +1443,7 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A29:A31"/>
+    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>